<commit_message>
create class and methods to retrieve data from yf
</commit_message>
<xml_diff>
--- a/df.xlsx
+++ b/df.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AVIO.MI" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TGYM.MI" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,65 +535,70 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>issuance_of_debt</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>operating_cash_flow</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>repayment_of_debt</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>repurchase_of_capital_stock</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>docs</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>diluted_eps</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>ebit</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>ebitda</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>gross_profit</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>net_income_common_stockholders</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>operating_income</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>pretax_income</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>tax_provision</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>total_revenue</t>
         </is>
@@ -602,7 +607,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AVIO.MI</t>
+          <t>TGYM.MI</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -614,34 +619,32 @@
         <v>44561</v>
       </c>
       <c r="D2" t="n">
-        <v>302479966</v>
+        <v>309841000</v>
       </c>
       <c r="E2" t="n">
-        <v>342276966</v>
+        <v>388938000</v>
       </c>
       <c r="F2" t="n">
-        <v>112122569</v>
+        <v>259145000</v>
       </c>
       <c r="G2" t="n">
-        <v>25688113</v>
+        <v>201327500</v>
       </c>
       <c r="H2" t="n">
-        <v>1236449960</v>
+        <v>763092000</v>
       </c>
       <c r="I2" t="n">
-        <v>324479966</v>
+        <v>322341000</v>
       </c>
       <c r="J2" t="n">
-        <v>47453797</v>
+        <v>103130000</v>
       </c>
       <c r="K2" t="n">
-        <v>926122736</v>
-      </c>
-      <c r="L2" t="n">
-        <v>671233</v>
-      </c>
+        <v>451531000</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>-9953662</v>
+        <v>124477000</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -649,66 +652,67 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>-33714000</v>
+        <v>-27691000</v>
       </c>
       <c r="P2" t="n">
-        <v>104615000</v>
+        <v>174306000</v>
       </c>
       <c r="Q2" t="n">
-        <v>-27594000</v>
+        <v>-127266000</v>
       </c>
       <c r="R2" t="n">
-        <v>7543000</v>
+        <v>65516000</v>
       </c>
       <c r="S2" t="n">
-        <v>-33714000</v>
+        <v>4323000</v>
       </c>
       <c r="T2" t="n">
-        <v>41257000</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>-10000000</v>
+        <v>93207000</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="inlineStr">
+        <v>-25000000</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr">
         <is>
           <t>income_stmt</t>
         </is>
       </c>
-      <c r="X2" t="n">
-        <v>0.32</v>
-      </c>
       <c r="Y2" t="n">
-        <v>8995135</v>
+        <v>0.31</v>
       </c>
       <c r="Z2" t="n">
-        <v>30146135</v>
+        <v>80598000</v>
       </c>
       <c r="AA2" t="n">
-        <v>96641887</v>
+        <v>117004000</v>
       </c>
       <c r="AB2" t="n">
-        <v>8479652</v>
+        <v>243759000</v>
       </c>
       <c r="AC2" t="n">
-        <v>5448628</v>
+        <v>63065000</v>
       </c>
       <c r="AD2" t="n">
-        <v>8622135</v>
+        <v>64185000</v>
       </c>
       <c r="AE2" t="n">
-        <v>-510378</v>
+        <v>79731000</v>
       </c>
       <c r="AF2" t="n">
-        <v>740983000</v>
+        <v>16466000</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>611412000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AVIO.MI</t>
+          <t>TGYM.MI</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -720,34 +724,32 @@
         <v>44926</v>
       </c>
       <c r="D3" t="n">
-        <v>293662323</v>
+        <v>343922000</v>
       </c>
       <c r="E3" t="n">
-        <v>343799323</v>
+        <v>375367000</v>
       </c>
       <c r="F3" t="n">
-        <v>109698831</v>
+        <v>288439000</v>
       </c>
       <c r="G3" t="n">
-        <v>25268139</v>
+        <v>201327500</v>
       </c>
       <c r="H3" t="n">
-        <v>1285356429</v>
+        <v>786207000</v>
       </c>
       <c r="I3" t="n">
-        <v>305738323</v>
+        <v>346547000</v>
       </c>
       <c r="J3" t="n">
-        <v>56952778</v>
+        <v>69220000</v>
       </c>
       <c r="K3" t="n">
-        <v>982095202</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1091207</v>
-      </c>
+        <v>440280000</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>-63916665</v>
+        <v>141471000</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -755,66 +757,69 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>-32515000</v>
+        <v>-34963000</v>
       </c>
       <c r="P3" t="n">
-        <v>131403000</v>
+        <v>205358000</v>
       </c>
       <c r="Q3" t="n">
-        <v>-4714000</v>
+        <v>-50795000</v>
       </c>
       <c r="R3" t="n">
-        <v>33224000</v>
+        <v>77280000</v>
       </c>
       <c r="S3" t="n">
-        <v>-34235000</v>
+        <v>-32112000</v>
       </c>
       <c r="T3" t="n">
-        <v>65739000</v>
+        <v>4006000</v>
       </c>
       <c r="U3" t="n">
-        <v>-10000000</v>
+        <v>112243000</v>
       </c>
       <c r="V3" t="n">
-        <v>-5739000</v>
-      </c>
-      <c r="W3" t="inlineStr">
+        <v>-54848000</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>income_stmt</t>
         </is>
       </c>
-      <c r="X3" t="n">
-        <v>-0.02</v>
-      </c>
       <c r="Y3" t="n">
-        <v>2266101</v>
+        <v>0.32</v>
       </c>
       <c r="Z3" t="n">
-        <v>21453101</v>
+        <v>84140000</v>
       </c>
       <c r="AA3" t="n">
-        <v>72403605</v>
+        <v>124504000</v>
       </c>
       <c r="AB3" t="n">
-        <v>-434767</v>
+        <v>278106000</v>
       </c>
       <c r="AC3" t="n">
-        <v>4605407</v>
+        <v>63587000</v>
       </c>
       <c r="AD3" t="n">
-        <v>1386101</v>
+        <v>82631000</v>
       </c>
       <c r="AE3" t="n">
-        <v>72425</v>
+        <v>83309000</v>
       </c>
       <c r="AF3" t="n">
-        <v>73218000</v>
+        <v>19434000</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>721490000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AVIO.MI</t>
+          <t>TGYM.MI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -826,34 +831,34 @@
         <v>45291</v>
       </c>
       <c r="D4" t="n">
-        <v>300616709</v>
+        <v>354544000</v>
       </c>
       <c r="E4" t="n">
-        <v>312711709</v>
+        <v>376629000</v>
       </c>
       <c r="F4" t="n">
-        <v>111565671</v>
+        <v>297859000</v>
       </c>
       <c r="G4" t="n">
-        <v>25268139</v>
+        <v>200490528</v>
       </c>
       <c r="H4" t="n">
-        <v>1055105106</v>
+        <v>818309000</v>
       </c>
       <c r="I4" t="n">
-        <v>302667709</v>
+        <v>354544000</v>
       </c>
       <c r="J4" t="n">
-        <v>19461650</v>
+        <v>65900000</v>
       </c>
       <c r="K4" t="n">
-        <v>744752387</v>
+        <v>454597000</v>
       </c>
       <c r="L4" t="n">
-        <v>1091207</v>
+        <v>836972</v>
       </c>
       <c r="M4" t="n">
-        <v>-98169676</v>
+        <v>158171000</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -861,64 +866,67 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>-36345000</v>
+        <v>-36179000</v>
       </c>
       <c r="P4" t="n">
-        <v>95593000</v>
+        <v>224730000</v>
       </c>
       <c r="Q4" t="n">
-        <v>-39441000</v>
+        <v>-50936000</v>
       </c>
       <c r="R4" t="n">
-        <v>6137000</v>
+        <v>70642000</v>
       </c>
       <c r="S4" t="n">
-        <v>-38850000</v>
-      </c>
-      <c r="T4" t="n">
-        <v>42482000</v>
-      </c>
-      <c r="U4" t="inlineStr"/>
+        <v>-30819000</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="n">
+        <v>106821000</v>
+      </c>
       <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="inlineStr">
+        <v>-11735000</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-6922000</v>
+      </c>
+      <c r="X4" t="inlineStr">
         <is>
           <t>income_stmt</t>
         </is>
       </c>
-      <c r="X4" t="n">
-        <v>0.25</v>
-      </c>
       <c r="Y4" t="n">
-        <v>7334048</v>
+        <v>0.37</v>
       </c>
       <c r="Z4" t="n">
-        <v>22617048</v>
+        <v>101142000</v>
       </c>
       <c r="AA4" t="n">
-        <v>111042799</v>
+        <v>146709000</v>
       </c>
       <c r="AB4" t="n">
-        <v>6487372</v>
+        <v>324677000</v>
       </c>
       <c r="AC4" t="n">
-        <v>2322936</v>
+        <v>73640000</v>
       </c>
       <c r="AD4" t="n">
-        <v>6641048</v>
+        <v>94699000</v>
       </c>
       <c r="AE4" t="n">
-        <v>17020</v>
+        <v>100400000</v>
       </c>
       <c r="AF4" t="n">
-        <v>35764000</v>
+        <v>23232000</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>808091000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AVIO.MI</t>
+          <t>TGYM.MI</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -930,34 +938,34 @@
         <v>45657</v>
       </c>
       <c r="D5" t="n">
-        <v>302826189</v>
+        <v>378996000</v>
       </c>
       <c r="E5" t="n">
-        <v>304880189</v>
+        <v>402722000</v>
       </c>
       <c r="F5" t="n">
-        <v>111240151</v>
+        <v>326301000</v>
       </c>
       <c r="G5" t="n">
-        <v>25268139</v>
+        <v>199161715</v>
       </c>
       <c r="H5" t="n">
-        <v>1092380164</v>
+        <v>904134000</v>
       </c>
       <c r="I5" t="n">
-        <v>302856189</v>
+        <v>378996000</v>
       </c>
       <c r="J5" t="n">
-        <v>11593526</v>
+        <v>70817000</v>
       </c>
       <c r="K5" t="n">
-        <v>779520040</v>
+        <v>517340000</v>
       </c>
       <c r="L5" t="n">
-        <v>1091207</v>
+        <v>2165785</v>
       </c>
       <c r="M5" t="n">
-        <v>-131067820</v>
+        <v>173773000</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -965,58 +973,59 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>-35161000</v>
+        <v>-41556000</v>
       </c>
       <c r="P5" t="n">
-        <v>101684000</v>
+        <v>268709000</v>
       </c>
       <c r="Q5" t="n">
-        <v>-19011000</v>
+        <v>-73019000</v>
       </c>
       <c r="R5" t="n">
-        <v>25101000</v>
+        <v>113852000</v>
       </c>
       <c r="S5" t="n">
-        <v>-35161000</v>
-      </c>
-      <c r="T5" t="n">
-        <v>60262000</v>
-      </c>
-      <c r="U5" t="inlineStr"/>
+        <v>-38611000</v>
+      </c>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="n">
+        <v>155408000</v>
+      </c>
       <c r="V5" t="n">
         <v>0</v>
       </c>
-      <c r="W5" t="inlineStr">
+      <c r="W5" t="n">
+        <v>-13128000</v>
+      </c>
+      <c r="X5" t="inlineStr">
         <is>
           <t>income_stmt</t>
         </is>
       </c>
-      <c r="X5" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>8390501</v>
-      </c>
+      <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="n">
-        <v>25826501</v>
+        <v>123883000</v>
       </c>
       <c r="AA5" t="n">
-        <v>132670549</v>
+        <v>175183000</v>
       </c>
       <c r="AB5" t="n">
-        <v>6087126</v>
+        <v>373496000</v>
       </c>
       <c r="AC5" t="n">
-        <v>5020014</v>
+        <v>87041000</v>
       </c>
       <c r="AD5" t="n">
-        <v>6763501</v>
+        <v>120940000</v>
       </c>
       <c r="AE5" t="n">
-        <v>378317</v>
+        <v>122962000</v>
       </c>
       <c r="AF5" t="n">
-        <v>312814000</v>
+        <v>33846000</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>901289000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>